<commit_message>
updating tempates for Resident Services
</commit_message>
<xml_diff>
--- a/_files/requirements/master_data/master-template_type.xlsx
+++ b/_files/requirements/master_data/master-template_type.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1045452\Documents\GitHub\mosip-docs.wiki\_files\requirements\master_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F419BDD4-C2A8-45B3-8856-E2FFB1DC2364}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D32213E3-12C5-48C1-BE7E-BEC5311DFF9A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1431" uniqueCount="369">
   <si>
     <t>code</t>
   </si>
@@ -632,6 +632,501 @@
   </si>
   <si>
     <t>RPR_MASKED_UIN_CARD_TEMPLATE</t>
+  </si>
+  <si>
+    <t>Authentication History Request Success Email</t>
+  </si>
+  <si>
+    <t>تاريخ طلب المصادقة</t>
+  </si>
+  <si>
+    <t>E-mail de réussite de la demande d'historique d'authentification</t>
+  </si>
+  <si>
+    <t>Authentication History Request Success SMS</t>
+  </si>
+  <si>
+    <t>تاريخ المصادقة طلب النجاح SMS</t>
+  </si>
+  <si>
+    <t>Historique de l'authentification des services résidents SMS de transcation</t>
+  </si>
+  <si>
+    <t>Authentication History Request Success EMAIL Subject</t>
+  </si>
+  <si>
+    <t>طلب سجل المصادقة النجاح عنوان البريد الإلكتروني</t>
+  </si>
+  <si>
+    <t>Succès EMAIL de la demande d'historique d'authentification</t>
+  </si>
+  <si>
+    <t>Successful Download of e-UIN Email</t>
+  </si>
+  <si>
+    <t>تنزيل ناجح للبريد الإلكتروني</t>
+  </si>
+  <si>
+    <t>Téléchargement réussi du courriel e-UIN</t>
+  </si>
+  <si>
+    <t>Successful Download of e-UIN Email Subject</t>
+  </si>
+  <si>
+    <t>تنزيل ناجح لموضوع البريد الإلكتروني UIN</t>
+  </si>
+  <si>
+    <t>Téléchargement réussi de l'objet de l'e-UIN</t>
+  </si>
+  <si>
+    <t>Successful Download of e-UIN SMS</t>
+  </si>
+  <si>
+    <t>تنزيل ناجح لرسائل e-UIN SMS</t>
+  </si>
+  <si>
+    <t>Téléchargement réussi de l'e-UIN SMS</t>
+  </si>
+  <si>
+    <t>Successful Locking of Auth Types Email</t>
+  </si>
+  <si>
+    <t>قفل ناجح لأنواع مصادقة البريد الإلكتروني</t>
+  </si>
+  <si>
+    <t>Verrouillage réussi des e-mails des types d'authentification</t>
+  </si>
+  <si>
+    <t>Successful Locking of Auth Types Email Subject</t>
+  </si>
+  <si>
+    <t>قفل ناجح لأنواع مصادقة البريد الإلكتروني الموضوع</t>
+  </si>
+  <si>
+    <t>Succès du verrouillage des types d'authentification</t>
+  </si>
+  <si>
+    <t>Successful Locking of Auth Types SMS</t>
+  </si>
+  <si>
+    <t>قفل ناجح لأنواع مصادقة الرسائل القصيرة</t>
+  </si>
+  <si>
+    <t>Verrouillage réussi des types d'authentification SMS</t>
+  </si>
+  <si>
+    <t>Successful Unlocking of Auth Types Email</t>
+  </si>
+  <si>
+    <t>فتح ناجح لأنواع مصادقة البريد الإلكتروني</t>
+  </si>
+  <si>
+    <t>Déverrouillage réussi des types d'authentification</t>
+  </si>
+  <si>
+    <t>Successful Unlocking of Auth Types Email Subject</t>
+  </si>
+  <si>
+    <t>فتح ناجح لأنواع مصادقة البريد الإلكتروني الموضوع</t>
+  </si>
+  <si>
+    <t>Déverrouillage réussi des types d'authentification Objet de l'e-mail</t>
+  </si>
+  <si>
+    <t>Successful Unlocking of Auth Types SMS</t>
+  </si>
+  <si>
+    <t>فتح ناجح لأنواع مصادقة الرسائل القصيرة</t>
+  </si>
+  <si>
+    <t>Déverrouillage réussi des types d'authentification SMS</t>
+  </si>
+  <si>
+    <t>VID Generation Success Email</t>
+  </si>
+  <si>
+    <t>VID جيل النجاح البريد الإلكتروني</t>
+  </si>
+  <si>
+    <t>E-mail de réussite de la génération VID</t>
+  </si>
+  <si>
+    <t>VID Generation Success Email Subject</t>
+  </si>
+  <si>
+    <t>VID جيل النجاح البريد الإلكتروني الموضوع</t>
+  </si>
+  <si>
+    <t>Sujet de l'e-mail de réussite de la génération VID</t>
+  </si>
+  <si>
+    <t>VID Generation Success SMS</t>
+  </si>
+  <si>
+    <t>VID جيل النجاح SMS</t>
+  </si>
+  <si>
+    <t>SMS de réussite de génération VID</t>
+  </si>
+  <si>
+    <t>VID Revocation Success Email</t>
+  </si>
+  <si>
+    <t>VID إبطال نجاح البريد الإلكتروني</t>
+  </si>
+  <si>
+    <t>E-mail de réussite de la révocation de VID</t>
+  </si>
+  <si>
+    <t>VID Revocation Success Email Subject</t>
+  </si>
+  <si>
+    <t>VID إبطال نجاح البريد الإلكتروني الموضوع</t>
+  </si>
+  <si>
+    <t>Sujet de l'e-mail de réussite de la révocation de VID</t>
+  </si>
+  <si>
+    <t>VID Revocation Success SMS</t>
+  </si>
+  <si>
+    <t>VID إبطال نجاح الرسائل القصيرة</t>
+  </si>
+  <si>
+    <t>SMS de succès de révocation VID</t>
+  </si>
+  <si>
+    <t>Reprint Request Success Email</t>
+  </si>
+  <si>
+    <t>طبع طلب النجاح البريد الإلكتروني</t>
+  </si>
+  <si>
+    <t>Réimpression de l'e-mail de réussite de la demande</t>
+  </si>
+  <si>
+    <t>Reprint Request Success Email Subject</t>
+  </si>
+  <si>
+    <t>طبع طلب النجاح البريد الإلكتروني الموضوع</t>
+  </si>
+  <si>
+    <t>Sujet de l'e-mail de demande de réimpression réussie</t>
+  </si>
+  <si>
+    <t>Reprint Request Success SMS</t>
+  </si>
+  <si>
+    <t>إعادة طبع طلب النجاح SMS</t>
+  </si>
+  <si>
+    <t>Réimpression SMS de réussite de la demande</t>
+  </si>
+  <si>
+    <t>Authentication History Request Failure Email</t>
+  </si>
+  <si>
+    <t>فشل طلب سجل المصادقة</t>
+  </si>
+  <si>
+    <t>E-mail d'échec de la demande d'historique d'authentification</t>
+  </si>
+  <si>
+    <t>Authentication History Request Failure Email Subject</t>
+  </si>
+  <si>
+    <t>Objet de l'e-mail d'échec de la demande d'historique d'authentification</t>
+  </si>
+  <si>
+    <t>Authentication History Request Failure SMS</t>
+  </si>
+  <si>
+    <t>SMS d'échec de la demande d'historique d'authentification</t>
+  </si>
+  <si>
+    <t>Download e-UIN Failure Email</t>
+  </si>
+  <si>
+    <t>تنزيل فشل البريد الإلكتروني</t>
+  </si>
+  <si>
+    <t>Télécharger l'e-mail d'échec e-UIN</t>
+  </si>
+  <si>
+    <t>Download e-UIN Failure Email Subject</t>
+  </si>
+  <si>
+    <t>قم بتنزيل موضوع فشل البريد الإلكتروني</t>
+  </si>
+  <si>
+    <t>Télécharger le sujet de l'e-mail d'échec e-UIN</t>
+  </si>
+  <si>
+    <t>Download e-UIN Failure SMS</t>
+  </si>
+  <si>
+    <t>قم بتنزيل SMS Failure SMS</t>
+  </si>
+  <si>
+    <t>Télécharger le SMS d'échec e-UIN</t>
+  </si>
+  <si>
+    <t>Failure in Locking of Auth Types Email</t>
+  </si>
+  <si>
+    <t>فشل في قفل البريد الإلكتروني لأنواع المصادقة</t>
+  </si>
+  <si>
+    <t>Échec du verrouillage des e-mails des types d'authentification</t>
+  </si>
+  <si>
+    <t>Failure in Locking of Auth Types Email Subject</t>
+  </si>
+  <si>
+    <t>فشل في قفل أنواع مصادقة البريد الإلكتروني الموضوع</t>
+  </si>
+  <si>
+    <t>Échec du verrouillage des types d'authentification Objet de l'e-mail</t>
+  </si>
+  <si>
+    <t>Failure in Locking of Auth Types SMS</t>
+  </si>
+  <si>
+    <t>فشل في قفل أنواع مصادقة الرسائل القصيرة</t>
+  </si>
+  <si>
+    <t>Échec du verrouillage des types d'authentification SMS</t>
+  </si>
+  <si>
+    <t>Reprint Request Failure Email</t>
+  </si>
+  <si>
+    <t>إعادة طبع فشل طلب البريد الإلكتروني</t>
+  </si>
+  <si>
+    <t>E-mail d'échec de la demande de réimpression</t>
+  </si>
+  <si>
+    <t>Reprint Request Failure Email Subject</t>
+  </si>
+  <si>
+    <t>Échec de la demande de réimpression Objet de l'e-mail</t>
+  </si>
+  <si>
+    <t>Reprint Request Failure SMS</t>
+  </si>
+  <si>
+    <t>إعادة طلب فشل الرسائل القصيرة</t>
+  </si>
+  <si>
+    <t>SMS d'échec de la demande de réimpression</t>
+  </si>
+  <si>
+    <t>Failure in Unlocking of Auth Types Email</t>
+  </si>
+  <si>
+    <t>فشل في فتح البريد الإلكتروني لأنواع مصادقة</t>
+  </si>
+  <si>
+    <t>Échec du déverrouillage de la messagerie électronique des types d'authentification</t>
+  </si>
+  <si>
+    <t>Failure in Unlocking of Auth Types Email Subject</t>
+  </si>
+  <si>
+    <t>فشل في فتح أنواع مصادقة البريد الإلكتروني الموضوع</t>
+  </si>
+  <si>
+    <t>Échec du déverrouillage du sujet de l'e-mail des types d'authentification</t>
+  </si>
+  <si>
+    <t>Failure in Unlocking of Auth Types SMS</t>
+  </si>
+  <si>
+    <t>فشل في فتح أنواع مصادقة الرسائل القصيرة</t>
+  </si>
+  <si>
+    <t>Échec de déverrouillage des types d'authentification SMS</t>
+  </si>
+  <si>
+    <t>VID Generation Failure Email</t>
+  </si>
+  <si>
+    <t>VID الجيل فشل البريد الإلكتروني</t>
+  </si>
+  <si>
+    <t>E-mail d'échec de génération de VID</t>
+  </si>
+  <si>
+    <t>VID Generation Failure Email Subject</t>
+  </si>
+  <si>
+    <t>VID الجيل فشل البريد الإلكتروني الموضوع</t>
+  </si>
+  <si>
+    <t>Objet de l'e-mail d'échec de génération de VID</t>
+  </si>
+  <si>
+    <t>VID Generation Failure SMS</t>
+  </si>
+  <si>
+    <t>فشل إنشاء VID SMS</t>
+  </si>
+  <si>
+    <t>SMS d'échec de génération de VID</t>
+  </si>
+  <si>
+    <t>VID Revocation Failure Email</t>
+  </si>
+  <si>
+    <t>VID إبطال فشل البريد الإلكتروني</t>
+  </si>
+  <si>
+    <t>E-mail d'échec de révocation de VID</t>
+  </si>
+  <si>
+    <t>VID Revocation Failure Email Subject</t>
+  </si>
+  <si>
+    <t>فيد إلغاء فشل البريد الإلكتروني الموضوع</t>
+  </si>
+  <si>
+    <t>Objet de l'e-mail d'échec de la révocation du VID</t>
+  </si>
+  <si>
+    <t>VID Revocation Failure SMS</t>
+  </si>
+  <si>
+    <t>فشل إلغاء VID SMS</t>
+  </si>
+  <si>
+    <t>SMS d'échec de révocation de VID</t>
+  </si>
+  <si>
+    <t>RS_AUTH_HIST_SUCCESS_EMAIL</t>
+  </si>
+  <si>
+    <t>RS_AUTH_HIST_SUCCESS_SMS</t>
+  </si>
+  <si>
+    <t>RS_AUTH_HIST_SUCCESS_EMAIL_SUB</t>
+  </si>
+  <si>
+    <t>RS_DOW_UIN_SUCCESS_EMAIL</t>
+  </si>
+  <si>
+    <t>RS_DOW_UIN_SUCCESS_EMAIL_SUB</t>
+  </si>
+  <si>
+    <t>RS_DOW_UIN_SUCCESS_SMS</t>
+  </si>
+  <si>
+    <t>RS_LOCK_AUTH_SUCCESS_EMAIL</t>
+  </si>
+  <si>
+    <t>RS_LOCK_AUTH_SUCCESS_EMAIL_SUB</t>
+  </si>
+  <si>
+    <t>RS_LOCK_AUTH_SUCCESS_SMS</t>
+  </si>
+  <si>
+    <t>RS_UNLOCK_AUTH_SUCCESS_EMAIL</t>
+  </si>
+  <si>
+    <t>RS_UNLOCK_AUTH_SUCCESS_EMAIL_SUB</t>
+  </si>
+  <si>
+    <t>RS_UNLOCK_AUTH_SUCCESS_SMS</t>
+  </si>
+  <si>
+    <t>RS_VIN_GEN_SUCCESS_EMAIL</t>
+  </si>
+  <si>
+    <t>RS_VIN_GEN_SUCCESS_EMAIL_SUB</t>
+  </si>
+  <si>
+    <t>RS_VIN_GEN_SUCCESS_SMS</t>
+  </si>
+  <si>
+    <t>RS_VIN_REV_SUCCESS_EMAIL</t>
+  </si>
+  <si>
+    <t>RS_VIN_REV_SUCCESS_EMAIL_SUB</t>
+  </si>
+  <si>
+    <t>RS_VIN_REV_SUCCESS_SMS</t>
+  </si>
+  <si>
+    <t>RS_UIN_RPR_SUCCESS_EMAIL</t>
+  </si>
+  <si>
+    <t>RS_UIN_RPR_SUCCESS_EMAIL_SUB</t>
+  </si>
+  <si>
+    <t>RS_UIN_RPR_SUCCESS_SMS</t>
+  </si>
+  <si>
+    <t>RS_AUTH_HIST_FAILURE_EMAIL</t>
+  </si>
+  <si>
+    <t>RS_AUTH_HIST_FAILURE_EMAIL_SUB</t>
+  </si>
+  <si>
+    <t>RS_AUTH_HIST_FAILURE_SMS</t>
+  </si>
+  <si>
+    <t>RS_DOW_UIN_FAILURE_EMAIL</t>
+  </si>
+  <si>
+    <t>RS_DOW_UIN_FAILURE_EMAIL_SUB</t>
+  </si>
+  <si>
+    <t>RS_DOW_UIN_FAILURE_SMS</t>
+  </si>
+  <si>
+    <t>RS_LOCK_AUTH_FAILURE_EMAIL</t>
+  </si>
+  <si>
+    <t>RS_LOCK_AUTH_FAILURE_EMAIL_SUB</t>
+  </si>
+  <si>
+    <t>RS_LOCK_AUTH_FAILURE_SMS</t>
+  </si>
+  <si>
+    <t>RS_UIN_RPR_FAILURE_EMAIL</t>
+  </si>
+  <si>
+    <t>RS_UIN_RPR_FAILURE_EMAIL_SUB</t>
+  </si>
+  <si>
+    <t>RS_UIN_RPR_FAILURE_SMS</t>
+  </si>
+  <si>
+    <t>RS_UNLOCK_AUTH_FAILURE_EMAIL</t>
+  </si>
+  <si>
+    <t>RS_UNLOCK_AUTH_FAILURE_EMAIL_SUB</t>
+  </si>
+  <si>
+    <t>RS_UNLOCK_AUTH_FAILURE_SMS</t>
+  </si>
+  <si>
+    <t>RS_VIN_GEN_FAILURE_EMAIL</t>
+  </si>
+  <si>
+    <t>RS_VIN_GEN_FAILURE_EMAIL_SUB</t>
+  </si>
+  <si>
+    <t>RS_VIN_GEN_FAILURE_SMS</t>
+  </si>
+  <si>
+    <t>RS_VIN_REV_FAILURE_EMAIL</t>
+  </si>
+  <si>
+    <t>RS_VIN_REV_FAILURE_EMAIL_SUB</t>
+  </si>
+  <si>
+    <t>RS_VIN_REV_FAILURE_SMS</t>
   </si>
 </sst>
 </file>
@@ -1115,9 +1610,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1473,10 +1971,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F160"/>
+  <dimension ref="A1:F286"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="A160" sqref="A160"/>
+    <sheetView tabSelected="1" topLeftCell="A277" workbookViewId="0">
+      <selection activeCell="A287" sqref="A287:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4686,6 +5184,2526 @@
         <v>10</v>
       </c>
     </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A161" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C161" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D161" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E161" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F161" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A162" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C162" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D162" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E162" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F162" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A163" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C163" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D163" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E163" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F163" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A164" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="B164" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C164" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D164" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E164" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F164" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A165" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="B165" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C165" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D165" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E165" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F165" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A166" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C166" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D166" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E166" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F166" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A167" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C167" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D167" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E167" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F167" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A168" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="B168" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C168" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D168" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E168" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F168" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A169" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="B169" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C169" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D169" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E169" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F169" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A170" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C170" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D170" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E170" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F170" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A171" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C171" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D171" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E171" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F171" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A172" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="B172" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C172" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D172" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E172" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F172" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A173" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="C173" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D173" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E173" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F173" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A174" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="B174" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C174" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D174" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E174" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F174" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A175" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="B175" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C175" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D175" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E175" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F175" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A176" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="B176" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C176" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D176" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E176" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F176" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A177" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C177" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D177" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E177" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F177" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A178" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C178" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D178" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E178" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F178" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A179" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="B179" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C179" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D179" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E179" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F179" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A180" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="B180" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C180" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D180" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E180" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F180" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A181" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="C181" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D181" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E181" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F181" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A182" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="B182" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C182" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D182" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E182" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F182" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A183" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C183" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D183" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E183" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F183" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A184" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="B184" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C184" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D184" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E184" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F184" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A185" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="B185" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C185" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D185" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E185" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F185" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A186" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="B186" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C186" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D186" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E186" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F186" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A187" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="B187" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C187" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D187" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E187" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F187" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A188" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B188" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C188" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D188" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E188" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F188" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A189" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B189" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C189" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D189" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E189" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F189" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A190" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B190" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C190" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D190" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E190" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F190" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A191" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="B191" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C191" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D191" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E191" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F191" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A192" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="B192" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C192" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D192" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E192" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F192" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A193" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="B193" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C193" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D193" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E193" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F193" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A194" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B194" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C194" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D194" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E194" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F194" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A195" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B195" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="C195" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D195" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E195" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F195" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A196" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B196" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C196" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D196" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E196" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F196" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A197" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="B197" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C197" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D197" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E197" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F197" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A198" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="B198" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C198" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D198" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E198" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F198" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A199" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="B199" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="C199" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D199" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E199" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F199" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A200" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="B200" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C200" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D200" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E200" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F200" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A201" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="B201" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C201" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D201" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E201" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F201" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A202" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="B202" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C202" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D202" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E202" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F202" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A203" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="B203" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="C203" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D203" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E203" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F203" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A204" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="B204" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C204" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D204" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E204" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F204" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A205" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="B205" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C205" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D205" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E205" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F205" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A206" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="B206" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C206" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D206" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E206" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F206" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A207" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="B207" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C207" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D207" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E207" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F207" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A208" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="B208" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="C208" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D208" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E208" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F208" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A209" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="B209" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C209" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D209" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E209" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F209" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A210" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="B210" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C210" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D210" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E210" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F210" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A211" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="B211" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="C211" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D211" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E211" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F211" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A212" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="B212" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="C212" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D212" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E212" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F212" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A213" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="B213" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="C213" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D213" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E213" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F213" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A214" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="B214" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="C214" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D214" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E214" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F214" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A215" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="B215" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="C215" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D215" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E215" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F215" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A216" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="B216" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="C216" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D216" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E216" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F216" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A217" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="B217" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C217" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D217" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E217" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F217" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A218" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="B218" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="C218" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D218" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E218" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F218" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A219" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="B219" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C219" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D219" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E219" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F219" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A220" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="B220" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C220" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D220" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E220" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F220" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A221" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="B221" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="C221" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D221" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E221" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F221" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A222" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="B222" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C222" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D222" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E222" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F222" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A223" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="B223" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C223" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D223" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E223" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F223" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A224" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="B224" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C224" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D224" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E224" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F224" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A225" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="B225" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C225" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D225" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E225" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F225" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A226" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="B226" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C226" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D226" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E226" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F226" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A227" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="B227" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="C227" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D227" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E227" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F227" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A228" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="B228" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C228" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D228" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E228" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F228" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A229" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="B229" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C229" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D229" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E229" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F229" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A230" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B230" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C230" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D230" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E230" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F230" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A231" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B231" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C231" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D231" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E231" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F231" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A232" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B232" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="C232" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D232" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E232" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F232" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A233" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="B233" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C233" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D233" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E233" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F233" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A234" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="B234" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C234" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D234" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E234" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F234" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A235" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="B235" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C235" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D235" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E235" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F235" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A236" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="B236" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C236" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D236" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E236" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F236" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A237" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="B237" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C237" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D237" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E237" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F237" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A238" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="B238" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="C238" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D238" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E238" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F238" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A239" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="B239" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="C239" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D239" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E239" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F239" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A240" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="B240" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="C240" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D240" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E240" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F240" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A241" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="B241" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="C241" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D241" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E241" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F241" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A242" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="B242" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C242" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D242" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E242" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F242" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A243" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="B243" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="C243" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D243" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E243" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F243" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A244" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="B244" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="C244" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D244" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E244" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F244" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A245" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B245" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="C245" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D245" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E245" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F245" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A246" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B246" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="C246" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D246" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E246" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F246" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A247" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B247" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C247" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D247" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E247" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F247" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A248" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B248" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="C248" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D248" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E248" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F248" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A249" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B249" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="C249" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D249" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E249" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F249" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="250" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A250" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B250" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="C250" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D250" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E250" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F250" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="251" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A251" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B251" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="C251" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D251" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E251" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F251" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="252" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A252" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B252" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="C252" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D252" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E252" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F252" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="253" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A253" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B253" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="C253" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D253" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E253" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F253" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="254" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A254" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B254" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="C254" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D254" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E254" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F254" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="255" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A255" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B255" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="C255" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D255" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E255" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F255" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="256" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A256" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B256" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="C256" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D256" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E256" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F256" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="257" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A257" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="B257" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="C257" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D257" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E257" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F257" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="258" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A258" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="B258" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="C258" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D258" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E258" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F258" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="259" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A259" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="B259" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="C259" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D259" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E259" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F259" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="260" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A260" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="B260" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="C260" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D260" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E260" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F260" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="261" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A261" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="B261" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="C261" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D261" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E261" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F261" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="262" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A262" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="B262" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="C262" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D262" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E262" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F262" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="263" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A263" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="B263" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="C263" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D263" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E263" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F263" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="264" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A264" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="B264" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="C264" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D264" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E264" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F264" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="265" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A265" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="B265" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="C265" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D265" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E265" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F265" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="266" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A266" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="B266" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="C266" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D266" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E266" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F266" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="267" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A267" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="B267" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="C267" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D267" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E267" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F267" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="268" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A268" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="B268" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="C268" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D268" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E268" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F268" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="269" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A269" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="B269" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C269" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D269" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E269" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F269" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="270" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A270" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="B270" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="C270" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D270" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E270" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F270" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="271" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A271" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="B271" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="C271" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D271" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E271" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F271" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="272" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A272" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="B272" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="C272" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D272" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E272" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F272" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="273" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A273" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="B273" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="C273" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D273" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E273" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F273" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="274" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A274" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="B274" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="C274" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D274" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E274" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F274" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="275" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A275" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="B275" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="C275" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D275" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E275" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F275" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="276" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A276" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="B276" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C276" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D276" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E276" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F276" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="277" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A277" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="B277" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="C277" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D277" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E277" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F277" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="278" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A278" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="B278" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="C278" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D278" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E278" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F278" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="279" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A279" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="B279" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="C279" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D279" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E279" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F279" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="280" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A280" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="B280" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="C280" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D280" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E280" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F280" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="281" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A281" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="B281" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="C281" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D281" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E281" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F281" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="282" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A282" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="B282" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="C282" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D282" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E282" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F282" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="283" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A283" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="B283" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="C283" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D283" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E283" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F283" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="284" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A284" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="B284" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="C284" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D284" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E284" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F284" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="285" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A285" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="B285" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="C285" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D285" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E285" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F285" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="286" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A286" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="B286" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="C286" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D286" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E286" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F286" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>